<commit_message>
urpavy kodu, premereni svalu 3
</commit_message>
<xml_diff>
--- a/Testovani/akce_levo_pravo.xlsx
+++ b/Testovani/akce_levo_pravo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MarekU\Škola\6.semester\Bakalarka\Testovani\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarekDarsaU\Documents\Škola\6.Semestr\Bakalarka\Testovani\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9DD3DD-60BE-478B-9AC7-A9FE30B1D04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A14B1F6-BCE3-472A-B619-279F4DA57518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3348" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Sval 1</t>
   </si>
@@ -51,15 +51,6 @@
   </si>
   <si>
     <t>Posun v krocích</t>
-  </si>
-  <si>
-    <t>Počáteční hodnota v mbar</t>
-  </si>
-  <si>
-    <t>Honota která by měla být v mbar</t>
-  </si>
-  <si>
-    <t>Hodnota která je v mbar</t>
   </si>
   <si>
     <t>Sval 2</t>
@@ -171,77 +162,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -548,13 +469,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D3:AC18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="4:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>0</v>
       </c>
@@ -570,17 +491,11 @@
       <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="M3" t="s">
         <v>5</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" t="s">
-        <v>8</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>1</v>
@@ -595,7 +510,7 @@
         <v>4</v>
       </c>
       <c r="S3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>1</v>
@@ -610,7 +525,7 @@
         <v>4</v>
       </c>
       <c r="Y3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Z3" s="1" t="s">
         <v>1</v>
@@ -625,7 +540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:29" x14ac:dyDescent="0.3">
       <c r="E4">
         <v>634</v>
       </c>
@@ -638,15 +553,6 @@
       <c r="H4">
         <v>7</v>
       </c>
-      <c r="I4">
-        <v>10</v>
-      </c>
-      <c r="J4">
-        <v>10.8</v>
-      </c>
-      <c r="K4">
-        <v>12</v>
-      </c>
       <c r="N4">
         <v>696</v>
       </c>
@@ -660,16 +566,16 @@
         <v>-28</v>
       </c>
       <c r="T4">
-        <v>635</v>
+        <v>648</v>
       </c>
       <c r="U4">
         <v>650</v>
       </c>
       <c r="V4" s="4">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="W4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Z4">
         <v>661</v>
@@ -684,7 +590,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="5" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:29" x14ac:dyDescent="0.3">
       <c r="E5">
         <f>G4</f>
         <v>652</v>
@@ -698,15 +604,6 @@
       <c r="H5">
         <v>21</v>
       </c>
-      <c r="I5">
-        <v>12</v>
-      </c>
-      <c r="J5">
-        <v>19.2</v>
-      </c>
-      <c r="K5">
-        <v>15</v>
-      </c>
       <c r="N5">
         <f>P4</f>
         <v>649</v>
@@ -722,16 +619,16 @@
       </c>
       <c r="T5">
         <f>V4</f>
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="U5">
         <v>700</v>
       </c>
       <c r="V5" s="4">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="W5">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="Z5">
         <f>AB4</f>
@@ -747,7 +644,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="6" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:29" x14ac:dyDescent="0.3">
       <c r="E6">
         <f t="shared" ref="E6:E10" si="0">G5</f>
         <v>673</v>
@@ -761,15 +658,6 @@
       <c r="H6">
         <v>12</v>
       </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>19.2</v>
-      </c>
-      <c r="K6">
-        <v>19</v>
-      </c>
       <c r="N6">
         <f t="shared" ref="N6:N10" si="1">P5</f>
         <v>639</v>
@@ -785,16 +673,16 @@
       </c>
       <c r="T6">
         <f t="shared" ref="T6:T10" si="2">V5</f>
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="U6">
         <v>700</v>
       </c>
       <c r="V6" s="4">
-        <v>715</v>
+        <v>706</v>
       </c>
       <c r="W6">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="Z6">
         <f t="shared" ref="Z6:Z10" si="3">AB5</f>
@@ -810,7 +698,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:29" x14ac:dyDescent="0.3">
       <c r="E7">
         <f t="shared" si="0"/>
         <v>687</v>
@@ -824,15 +712,6 @@
       <c r="H7">
         <v>-26</v>
       </c>
-      <c r="I7">
-        <v>19</v>
-      </c>
-      <c r="J7">
-        <v>7.4</v>
-      </c>
-      <c r="K7">
-        <v>11</v>
-      </c>
       <c r="N7">
         <f t="shared" si="1"/>
         <v>629</v>
@@ -848,13 +727,13 @@
       </c>
       <c r="T7">
         <f t="shared" si="2"/>
-        <v>715</v>
+        <v>706</v>
       </c>
       <c r="U7">
         <v>630</v>
       </c>
       <c r="V7" s="4">
-        <v>662</v>
+        <v>685</v>
       </c>
       <c r="W7">
         <v>-52</v>
@@ -873,7 +752,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:29" x14ac:dyDescent="0.3">
       <c r="E8">
         <f t="shared" si="0"/>
         <v>674</v>
@@ -887,15 +766,6 @@
       <c r="H8">
         <v>-20</v>
       </c>
-      <c r="I8">
-        <v>11</v>
-      </c>
-      <c r="J8">
-        <v>7.4</v>
-      </c>
-      <c r="K8">
-        <v>9</v>
-      </c>
       <c r="N8">
         <f t="shared" si="1"/>
         <v>646</v>
@@ -911,13 +781,13 @@
       </c>
       <c r="T8">
         <f t="shared" si="2"/>
-        <v>662</v>
+        <v>685</v>
       </c>
       <c r="U8">
         <v>630</v>
       </c>
-      <c r="V8">
-        <v>636</v>
+      <c r="V8" s="4">
+        <v>645</v>
       </c>
       <c r="W8">
         <v>-20</v>
@@ -936,7 +806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:29" x14ac:dyDescent="0.3">
       <c r="E9">
         <f t="shared" si="0"/>
         <v>628</v>
@@ -944,19 +814,10 @@
       <c r="F9">
         <v>650</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="4">
         <v>639</v>
       </c>
       <c r="H9">
-        <v>10</v>
-      </c>
-      <c r="I9">
-        <v>9</v>
-      </c>
-      <c r="J9">
-        <v>10.8</v>
-      </c>
-      <c r="K9">
         <v>10</v>
       </c>
       <c r="N9">
@@ -974,13 +835,13 @@
       </c>
       <c r="T9">
         <f t="shared" si="2"/>
-        <v>636</v>
+        <v>645</v>
       </c>
       <c r="U9">
         <v>650</v>
       </c>
       <c r="V9" s="4">
-        <v>636</v>
+        <v>642</v>
       </c>
       <c r="W9">
         <v>8</v>
@@ -999,7 +860,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="10" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:29" x14ac:dyDescent="0.3">
       <c r="E10">
         <f t="shared" si="0"/>
         <v>639</v>
@@ -1007,17 +868,11 @@
       <c r="F10">
         <v>650</v>
       </c>
+      <c r="G10" s="4">
+        <v>653</v>
+      </c>
       <c r="H10">
         <v>5</v>
-      </c>
-      <c r="I10">
-        <v>10</v>
-      </c>
-      <c r="J10">
-        <v>10.8</v>
-      </c>
-      <c r="K10">
-        <v>12</v>
       </c>
       <c r="N10">
         <f t="shared" si="1"/>
@@ -1026,15 +881,21 @@
       <c r="O10">
         <v>650</v>
       </c>
+      <c r="P10" s="4">
+        <v>641</v>
+      </c>
       <c r="Q10">
         <v>-27</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>636</v>
+        <v>642</v>
       </c>
       <c r="U10">
         <v>650</v>
+      </c>
+      <c r="V10" s="4">
+        <v>647</v>
       </c>
       <c r="W10">
         <v>8</v>
@@ -1046,34 +907,37 @@
       <c r="AA10">
         <v>650</v>
       </c>
+      <c r="AB10">
+        <v>642</v>
+      </c>
       <c r="AC10">
         <v>-2</v>
       </c>
     </row>
-    <row r="18" spans="23:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="23:23" x14ac:dyDescent="0.3">
       <c r="W18" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G4:G9">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="between">
+  <conditionalFormatting sqref="G4:G10">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="between">
       <formula>$F4-10</formula>
       <formula>$F4+10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P10">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
       <formula>$O4-10</formula>
       <formula>$O4+10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4:V10">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>$U4-10</formula>
       <formula>$U4+10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB4:AB10">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>$AA4-10</formula>
       <formula>$AA4+10</formula>
     </cfRule>

</xml_diff>

<commit_message>
dodělano testovani, diskuze a závěr + fin upravy
</commit_message>
<xml_diff>
--- a/Testovani/akce_levo_pravo.xlsx
+++ b/Testovani/akce_levo_pravo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarekDarsaU\Documents\Škola\6.Semestr\Bakalarka\Testovani\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MarekU\Škola\6.semester\Bakalarka\Testovani\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D0FD09-9E3C-4B09-94E6-E447C76E7FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AA0A44-054E-4009-9C74-949515D945BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -44,12 +44,6 @@
     <t>Počáteční hodnota v mV</t>
   </si>
   <si>
-    <t>Honota která by měla být v mV</t>
-  </si>
-  <si>
-    <t>Hodnota která je v mV</t>
-  </si>
-  <si>
     <t>Posun v krocích</t>
   </si>
   <si>
@@ -61,12 +55,18 @@
   <si>
     <t>Sval 4</t>
   </si>
+  <si>
+    <t>Hodnota, která by měla být v mV</t>
+  </si>
+  <si>
+    <t>Hodnota, která je v mV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,8 +82,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,8 +109,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -121,17 +134,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="4"/>
-      </right>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="4"/>
       </left>
@@ -142,11 +144,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF5B9BD5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF5B9BD5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF5B9BD5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -154,10 +176,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,80 +495,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D3:AC18"/>
+  <dimension ref="A2:AC18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="4:29" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
+    <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="M3" t="s">
+      <c r="L3" s="4"/>
+      <c r="M3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="Z3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="AA3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="4" spans="4:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E4">
         <v>634</v>
       </c>
@@ -571,8 +606,8 @@
       <c r="U4">
         <v>650</v>
       </c>
-      <c r="V4" s="4">
-        <v>637</v>
+      <c r="V4" s="3">
+        <v>647</v>
       </c>
       <c r="W4">
         <v>0</v>
@@ -590,7 +625,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="5" spans="4:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E5">
         <f>G4</f>
         <v>652</v>
@@ -598,7 +633,7 @@
       <c r="F5">
         <v>700</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>673</v>
       </c>
       <c r="H5">
@@ -619,16 +654,16 @@
       </c>
       <c r="T5">
         <f>V4</f>
-        <v>637</v>
+        <v>647</v>
       </c>
       <c r="U5">
         <v>700</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5" s="3">
         <v>664</v>
       </c>
       <c r="W5">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="Z5">
         <f>AB4</f>
@@ -644,7 +679,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="6" spans="4:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E6">
         <f t="shared" ref="E6:E10" si="0">G5</f>
         <v>673</v>
@@ -652,7 +687,7 @@
       <c r="F6">
         <v>700</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>691</v>
       </c>
       <c r="H6">
@@ -678,7 +713,7 @@
       <c r="U6">
         <v>700</v>
       </c>
-      <c r="V6" s="4">
+      <c r="V6" s="3">
         <v>706</v>
       </c>
       <c r="W6">
@@ -698,7 +733,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="4:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E7">
         <f t="shared" si="0"/>
         <v>691</v>
@@ -706,7 +741,7 @@
       <c r="F7">
         <v>630</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>674</v>
       </c>
       <c r="H7">
@@ -719,7 +754,7 @@
       <c r="O7">
         <v>700</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="3">
         <v>646</v>
       </c>
       <c r="Q7">
@@ -732,7 +767,7 @@
       <c r="U7">
         <v>630</v>
       </c>
-      <c r="V7" s="4">
+      <c r="V7" s="3">
         <v>685</v>
       </c>
       <c r="W7">
@@ -752,7 +787,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="4:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E8">
         <f t="shared" si="0"/>
         <v>674</v>
@@ -786,7 +821,7 @@
       <c r="U8">
         <v>630</v>
       </c>
-      <c r="V8" s="4">
+      <c r="V8" s="3">
         <v>645</v>
       </c>
       <c r="W8">
@@ -806,7 +841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="4:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E9">
         <f t="shared" si="0"/>
         <v>628</v>
@@ -814,7 +849,7 @@
       <c r="F9">
         <v>650</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>639</v>
       </c>
       <c r="H9">
@@ -827,7 +862,7 @@
       <c r="O9">
         <v>650</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="3">
         <v>695</v>
       </c>
       <c r="Q9">
@@ -840,7 +875,7 @@
       <c r="U9">
         <v>650</v>
       </c>
-      <c r="V9" s="4">
+      <c r="V9" s="3">
         <v>642</v>
       </c>
       <c r="W9">
@@ -860,7 +895,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="10" spans="4:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E10">
         <f t="shared" si="0"/>
         <v>639</v>
@@ -868,7 +903,7 @@
       <c r="F10">
         <v>650</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>653</v>
       </c>
       <c r="H10">
@@ -881,7 +916,7 @@
       <c r="O10">
         <v>650</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10" s="3">
         <v>641</v>
       </c>
       <c r="Q10">
@@ -894,7 +929,7 @@
       <c r="U10">
         <v>650</v>
       </c>
-      <c r="V10" s="4">
+      <c r="V10" s="3">
         <v>647</v>
       </c>
       <c r="W10">
@@ -914,8 +949,8 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="18" spans="23:23" x14ac:dyDescent="0.3">
-      <c r="W18" s="4"/>
+    <row r="18" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W18" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G4:G10">

</xml_diff>